<commit_message>
feat: raw excel line items list created
</commit_message>
<xml_diff>
--- a/template/new-excel-template.xlsx
+++ b/template/new-excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ifinworth\ifinworth\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30594CD1-E9E1-4F92-884B-2203CD4EBD3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23110870-A8A3-46C5-A7C6-5396F1ED24A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{B1689DFF-EE47-4FC0-B162-7D2AF1E3E42F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
   <si>
     <t>Income</t>
   </si>
@@ -223,9 +223,6 @@
     <t>(a) Equity share capital</t>
   </si>
   <si>
-    <t>(b) other equity</t>
-  </si>
-  <si>
     <t>Total Equity</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>Total Equity and Liabilities</t>
   </si>
   <si>
-    <t>Equity Infusion</t>
-  </si>
-  <si>
     <t>(ii) revaluation Reserve</t>
   </si>
   <si>
@@ -425,6 +419,18 @@
   </si>
   <si>
     <t>(ii) other financial liabilities</t>
+  </si>
+  <si>
+    <t>(b) Preference share capital</t>
+  </si>
+  <si>
+    <t>(c) Equity Infusion</t>
+  </si>
+  <si>
+    <t>(d) Share Application Money Pending Allotment</t>
+  </si>
+  <si>
+    <t>(e) other equity</t>
   </si>
 </sst>
 </file>
@@ -709,8 +715,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}" name="Table2" displayName="Table2" ref="A1:B74" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:B74" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}" name="Table2" displayName="Table2" ref="A1:B76" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:B76" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{29F1FAD9-78DC-41FD-A936-34B0C5D691FA}" name="Particulars"/>
     <tableColumn id="3" xr3:uid="{9DBBC197-E070-4701-8D24-C4BA3A4E441B}" name="{{Add Provisional financial date in DD-MM-YYYY}} format" dataDxfId="0" dataCellStyle="Currency"/>
@@ -1058,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6">
@@ -1072,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="10"/>
     </row>
@@ -1081,7 +1087,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" s="10"/>
     </row>
@@ -1090,10 +1096,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" s="25">
         <f>SUM(C7:C14)</f>
@@ -1120,13 +1126,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C11" s="11"/>
     </row>
@@ -1138,14 +1144,14 @@
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="14.4" thickBot="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="10"/>
     </row>
@@ -1187,7 +1193,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="10"/>
     </row>
@@ -1199,7 +1205,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="B22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="10"/>
     </row>
@@ -1208,7 +1214,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="B24" s="44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C24" s="47">
         <f>SUM(C25:C27)</f>
@@ -1217,19 +1223,19 @@
     </row>
     <row r="25" spans="1:3">
       <c r="B25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3">
       <c r="B26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C27" s="11"/>
     </row>
@@ -1239,7 +1245,7 @@
     <row r="29" spans="1:3" s="1" customFormat="1" ht="14.4" thickBot="1">
       <c r="A29" s="37"/>
       <c r="B29" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C29" s="38">
         <f>SUM(C18:C22)+C24</f>
@@ -1254,7 +1260,7 @@
     <row r="31" spans="1:3" s="1" customFormat="1" ht="27.6">
       <c r="A31" s="7"/>
       <c r="B31" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C31" s="26">
         <f t="shared" ref="C31" si="0">C15-C29</f>
@@ -1264,7 +1270,7 @@
     <row r="32" spans="1:3" s="1" customFormat="1">
       <c r="A32"/>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="19"/>
     </row>
@@ -1274,7 +1280,7 @@
     <row r="34" spans="1:3">
       <c r="A34" s="7"/>
       <c r="B34" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C34" s="26">
         <f>C31-C32</f>
@@ -1295,7 +1301,7 @@
         <v>14</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C37" s="26">
         <f>C34-C35</f>
@@ -1319,7 +1325,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C40" s="26">
         <f>C37-C38</f>
@@ -1356,7 +1362,7 @@
     <row r="45" spans="1:3" s="1" customFormat="1" ht="14.4" thickBot="1">
       <c r="A45" s="39"/>
       <c r="B45" s="39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C45" s="40">
         <f>SUM(C43:C44)</f>
@@ -1406,7 +1412,7 @@
         <v>27</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C51" s="26">
         <f>C49-C50</f>
@@ -1461,13 +1467,13 @@
     </row>
     <row r="59" spans="1:3">
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C59" s="11"/>
     </row>
     <row r="60" spans="1:3" ht="27.6">
       <c r="B60" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C60" s="11"/>
     </row>
@@ -1479,13 +1485,13 @@
     </row>
     <row r="62" spans="1:3">
       <c r="B62" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C62" s="11"/>
     </row>
     <row r="63" spans="1:3" ht="27.6">
       <c r="B63" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C63" s="11"/>
     </row>
@@ -1497,7 +1503,7 @@
         <v>34</v>
       </c>
       <c r="B65" s="41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C65" s="38">
         <f>C53+SUM(C59:C63)</f>
@@ -1525,7 +1531,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A18FAD7-F36A-4E9F-A54A-A2283D8CD4A4}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -1542,7 +1548,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.399999999999999">
@@ -1563,7 +1569,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" s="12"/>
     </row>
@@ -1605,7 +1611,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" s="18"/>
     </row>
@@ -1629,25 +1635,25 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B16" s="18"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B17" s="18"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" s="18"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B19" s="18"/>
     </row>
@@ -1659,13 +1665,13 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B21" s="22"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B22" s="22"/>
     </row>
@@ -1675,7 +1681,7 @@
     </row>
     <row r="24" spans="1:2" ht="16.2" thickBot="1">
       <c r="A24" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="49">
         <f t="shared" ref="B24" si="0">SUM(B6:B14,B16:B22)</f>
@@ -1706,7 +1712,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B29" s="18"/>
     </row>
@@ -1730,7 +1736,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" s="18"/>
     </row>
@@ -1794,216 +1800,228 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="11"/>
+        <v>131</v>
+      </c>
+      <c r="B44" s="12"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B45" s="11"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="14"/>
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="11"/>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="15" t="s">
-        <v>85</v>
+      <c r="A47" t="s">
+        <v>134</v>
       </c>
       <c r="B47" s="11"/>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="11"/>
-    </row>
-    <row r="49" spans="1:2" ht="14.4" thickBot="1">
-      <c r="A49" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="30"/>
-    </row>
-    <row r="50" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A50" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="14"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="11"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="11"/>
+    </row>
+    <row r="51" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A51" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="30"/>
+    </row>
+    <row r="52" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A52" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="49">
+        <f>SUM(B43:B51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.6">
+      <c r="A53" s="2"/>
+      <c r="B53" s="11"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6">
+      <c r="A54" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="49">
-        <f>SUM(B43:B49)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.6">
-      <c r="A51" s="2"/>
-      <c r="B51" s="11"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.6">
-      <c r="A52" s="2" t="s">
+      <c r="B54" s="11"/>
+    </row>
+    <row r="55" spans="1:2" ht="15.6">
+      <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="11"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6">
-      <c r="A53" s="2" t="s">
+      <c r="B55" s="11"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="11"/>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+      <c r="B56" s="12"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="12"/>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="15" t="s">
+      <c r="B57" s="18"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="18"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="18"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="18"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="18"/>
+    </row>
+    <row r="62" spans="1:2" ht="30" customHeight="1">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="22"/>
+    </row>
+    <row r="63" spans="1:2" ht="30" customHeight="1" thickBot="1">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="22"/>
+    </row>
+    <row r="64" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A64" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B64" s="48">
+        <f>SUM(B57:B63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.6">
+      <c r="A65" s="2"/>
+      <c r="B65" s="11"/>
+    </row>
+    <row r="66" spans="1:2" ht="15.6">
+      <c r="A66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="11"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="11"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" s="18"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="18"/>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" s="18"/>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B57" s="18"/>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="18"/>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>73</v>
-      </c>
-      <c r="B59" s="18"/>
-    </row>
-    <row r="60" spans="1:2" ht="30" customHeight="1">
-      <c r="A60" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="22"/>
-    </row>
-    <row r="61" spans="1:2" ht="30" customHeight="1" thickBot="1">
-      <c r="A61" t="s">
-        <v>106</v>
-      </c>
-      <c r="B61" s="22"/>
-    </row>
-    <row r="62" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A62" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B62" s="48">
-        <f>SUM(B55:B61)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="15.6">
-      <c r="A63" s="2"/>
-      <c r="B63" s="11"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.6">
-      <c r="A64" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B64" s="11"/>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="11"/>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="15" t="s">
+      <c r="B69" s="18"/>
+    </row>
+    <row r="70" spans="1:2" ht="27.6">
+      <c r="A70" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="18"/>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="18"/>
-    </row>
-    <row r="68" spans="1:2" ht="27.6">
-      <c r="A68" s="20" t="s">
+      <c r="B70" s="18"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="18"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
+      <c r="B71" s="18"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
         <v>79</v>
       </c>
-      <c r="B69" s="18"/>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
+      <c r="B72" s="18"/>
+    </row>
+    <row r="73" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A73" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="18"/>
-    </row>
-    <row r="71" spans="1:2" ht="14.4" thickBot="1">
-      <c r="A71" s="32" t="s">
+      <c r="B73" s="22"/>
+    </row>
+    <row r="74" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A74" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="22"/>
-    </row>
-    <row r="72" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A72" s="35" t="s">
+      <c r="B74" s="37">
+        <f t="shared" ref="B74" si="2">SUM(B68:B73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A75" s="33"/>
+      <c r="B75" s="13"/>
+    </row>
+    <row r="76" spans="1:2" ht="18" thickBot="1">
+      <c r="A76" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="37">
-        <f t="shared" ref="B72" si="2">SUM(B66:B71)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A73" s="33"/>
-      <c r="B73" s="13"/>
-    </row>
-    <row r="74" spans="1:2" ht="18" thickBot="1">
-      <c r="A74" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" s="49">
-        <f t="shared" ref="B74" si="3">SUM(B50,B62,B72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="15.6">
-      <c r="A76" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="B76" s="50">
-        <f>IF(B74=B38,0,B38-B74)</f>
+      <c r="B76" s="49">
+        <f>SUM(B52,B64,B74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.6">
+      <c r="A78" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B78" s="50">
+        <f>IF(B76=B38,0,B38-B76)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" pivotTables="0"/>
   <protectedRanges>
-    <protectedRange sqref="B44:B48 B65 B54 B5:B6 B15 B11 B13 B26" name="Range1"/>
+    <protectedRange sqref="B45:B50 B67 B56 B5:B6 B15 B11 B13 B26" name="Range1"/>
     <protectedRange sqref="B7:B10" name="Range1_2"/>
     <protectedRange sqref="B12" name="Range1_3"/>
     <protectedRange sqref="B16:B17" name="Range1_5"/>
     <protectedRange sqref="B18:B23" name="Range1_6"/>
     <protectedRange sqref="B27:B30" name="Range1_7"/>
-    <protectedRange sqref="B57:B61" name="Range1_15"/>
-    <protectedRange sqref="B66:B67" name="Range1_16"/>
+    <protectedRange sqref="B59:B63" name="Range1_15"/>
+    <protectedRange sqref="B68:B69" name="Range1_16"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat:Immovable subclassification (Plant and Machinary and Land and Buildings) added
</commit_message>
<xml_diff>
--- a/template/new-excel-template.xlsx
+++ b/template/new-excel-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ifinworth\ifinworth\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23110870-A8A3-46C5-A7C6-5396F1ED24A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5545C6B4-4D0B-481B-B5D1-479B550D6A48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{B1689DFF-EE47-4FC0-B162-7D2AF1E3E42F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t>Income</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t>(e) other equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Land &amp; Building</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Plant &amp; Machinery</t>
   </si>
 </sst>
 </file>
@@ -715,8 +721,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}" name="Table2" displayName="Table2" ref="A1:B76" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:B76" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}" name="Table2" displayName="Table2" ref="A1:B78" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:B78" xr:uid="{9575A952-4FE5-4169-A062-272B3805781E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{29F1FAD9-78DC-41FD-A936-34B0C5D691FA}" name="Particulars"/>
     <tableColumn id="3" xr3:uid="{9DBBC197-E070-4701-8D24-C4BA3A4E441B}" name="{{Add Provisional financial date in DD-MM-YYYY}} format" dataDxfId="0" dataCellStyle="Currency"/>
@@ -1531,7 +1537,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A18FAD7-F36A-4E9F-A54A-A2283D8CD4A4}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -1586,442 +1592,454 @@
       <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="18"/>
+      <c r="A8" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="18"/>
+      <c r="A9" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="18"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B11" s="18"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="B12" s="18"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="18"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="18"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="16" t="s">
+      <c r="B16" s="18"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="18"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="12"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="15" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B18" s="18"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="18"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="18"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="18"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="16" t="s">
+      <c r="B21" s="18"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="23" t="s">
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="15" t="s">
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:2" ht="14.4" thickBot="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A24" s="31" t="s">
+      <c r="B24" s="22"/>
+    </row>
+    <row r="25" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A25" s="15"/>
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A26" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="49">
-        <f t="shared" ref="B24" si="0">SUM(B6:B14,B16:B22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.6">
-      <c r="A25" s="2"/>
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.6">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="49">
+        <f>SUM(B6:B16,B18:B24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.6">
+      <c r="A27" s="2"/>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.6">
+      <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="11"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="18"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="B29" s="18"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>55</v>
-      </c>
-      <c r="B28" s="18"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="18"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="B30" s="18"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="15" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="B31" s="18"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B32" s="18"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="15" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="B33" s="18"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="18"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="18"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="18"/>
-    </row>
-    <row r="35" spans="1:2" ht="14.4" thickBot="1">
-      <c r="A35" t="s">
+      <c r="B36" s="18"/>
+    </row>
+    <row r="37" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A37" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A36" s="31" t="s">
+      <c r="B37" s="22"/>
+    </row>
+    <row r="38" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A38" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="49">
-        <f>SUM(B27,B29:B35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="13"/>
-    </row>
-    <row r="38" spans="1:2" ht="18" thickBot="1">
-      <c r="A38" s="9" t="s">
+      <c r="B38" s="49">
+        <f>SUM(B29,B31:B37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A39" s="33"/>
+      <c r="B39" s="13"/>
+    </row>
+    <row r="40" spans="1:2" ht="18" thickBot="1">
+      <c r="A40" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="49">
-        <f t="shared" ref="B38" si="1">SUM(B24,B36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="B39" s="11"/>
-    </row>
-    <row r="40" spans="1:2" ht="17.399999999999999">
-      <c r="A40" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="11"/>
+      <c r="B40" s="49">
+        <f t="shared" ref="B40" si="0">SUM(B26,B38)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
       <c r="B41" s="11"/>
     </row>
-    <row r="42" spans="1:2" ht="15.6">
-      <c r="A42" s="2" t="s">
+    <row r="42" spans="1:2" ht="17.399999999999999">
+      <c r="A42" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="11"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:2" ht="15.6">
+      <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="11"/>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="18"/>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>131</v>
-      </c>
-      <c r="B44" s="12"/>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>132</v>
-      </c>
-      <c r="B45" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="B45" s="18"/>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>133</v>
-      </c>
-      <c r="B46" s="11"/>
+        <v>131</v>
+      </c>
+      <c r="B46" s="12"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="11"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="11"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>134</v>
-      </c>
-      <c r="B47" s="11"/>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="14"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="B49" s="11"/>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="14"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="11"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="11"/>
-    </row>
-    <row r="51" spans="1:2" ht="14.4" thickBot="1">
-      <c r="A51" s="29" t="s">
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A53" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="30"/>
-    </row>
-    <row r="52" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A52" s="31" t="s">
+      <c r="B53" s="30"/>
+    </row>
+    <row r="54" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A54" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="49">
-        <f>SUM(B43:B51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.6">
-      <c r="A53" s="2"/>
-      <c r="B53" s="11"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.6">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="49">
+        <f>SUM(B45:B53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.6">
+      <c r="A55" s="2"/>
+      <c r="B55" s="11"/>
+    </row>
+    <row r="56" spans="1:2" ht="15.6">
+      <c r="A56" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="11"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.6">
-      <c r="A55" s="2" t="s">
+      <c r="B56" s="11"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.6">
+      <c r="A57" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="11"/>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+      <c r="B57" s="11"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="12"/>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="15" t="s">
+      <c r="B58" s="12"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="18"/>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="20" t="s">
+      <c r="B59" s="18"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="18"/>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="20" t="s">
+      <c r="B60" s="18"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="18"/>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+      <c r="B61" s="18"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="18"/>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+      <c r="B62" s="18"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="18"/>
-    </row>
-    <row r="62" spans="1:2" ht="30" customHeight="1">
-      <c r="A62" t="s">
+      <c r="B63" s="18"/>
+    </row>
+    <row r="64" spans="1:2" ht="30" customHeight="1">
+      <c r="A64" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="22"/>
-    </row>
-    <row r="63" spans="1:2" ht="30" customHeight="1" thickBot="1">
-      <c r="A63" t="s">
+      <c r="B64" s="22"/>
+    </row>
+    <row r="65" spans="1:2" ht="30" customHeight="1" thickBot="1">
+      <c r="A65" t="s">
         <v>104</v>
       </c>
-      <c r="B63" s="22"/>
-    </row>
-    <row r="64" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A64" s="35" t="s">
+      <c r="B65" s="22"/>
+    </row>
+    <row r="66" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A66" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="48">
-        <f>SUM(B57:B63)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="15.6">
-      <c r="A65" s="2"/>
-      <c r="B65" s="11"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.6">
-      <c r="A66" s="2" t="s">
+      <c r="B66" s="48">
+        <f>SUM(B59:B65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.6">
+      <c r="A67" s="2"/>
+      <c r="B67" s="11"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.6">
+      <c r="A68" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="11"/>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+      <c r="B68" s="11"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
         <v>75</v>
       </c>
-      <c r="B67" s="11"/>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="15" t="s">
+      <c r="B69" s="11"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B68" s="18"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="15" t="s">
+      <c r="B70" s="18"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="18"/>
-    </row>
-    <row r="70" spans="1:2" ht="27.6">
-      <c r="A70" s="20" t="s">
+      <c r="B71" s="18"/>
+    </row>
+    <row r="72" spans="1:2" ht="27.6">
+      <c r="A72" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="18"/>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
+      <c r="B72" s="18"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="18"/>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
+      <c r="B73" s="18"/>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>79</v>
       </c>
-      <c r="B72" s="18"/>
-    </row>
-    <row r="73" spans="1:2" ht="14.4" thickBot="1">
-      <c r="A73" s="32" t="s">
+      <c r="B74" s="18"/>
+    </row>
+    <row r="75" spans="1:2" ht="14.4" thickBot="1">
+      <c r="A75" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="22"/>
-    </row>
-    <row r="74" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A74" s="35" t="s">
+      <c r="B75" s="22"/>
+    </row>
+    <row r="76" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A76" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="37">
-        <f t="shared" ref="B74" si="2">SUM(B68:B73)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A75" s="33"/>
-      <c r="B75" s="13"/>
-    </row>
-    <row r="76" spans="1:2" ht="18" thickBot="1">
-      <c r="A76" s="9" t="s">
+      <c r="B76" s="37">
+        <f t="shared" ref="B76" si="1">SUM(B70:B75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A77" s="33"/>
+      <c r="B77" s="13"/>
+    </row>
+    <row r="78" spans="1:2" ht="18" thickBot="1">
+      <c r="A78" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B76" s="49">
-        <f>SUM(B52,B64,B74)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="15.6">
-      <c r="A78" s="34" t="s">
+      <c r="B78" s="49">
+        <f>SUM(B54,B66,B76)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.6">
+      <c r="A80" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B78" s="50">
-        <f>IF(B76=B38,0,B38-B76)</f>
+      <c r="B80" s="50">
+        <f>IF(B78=B40,0,B40-B78)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" pivotTables="0"/>
   <protectedRanges>
-    <protectedRange sqref="B45:B50 B67 B56 B5:B6 B15 B11 B13 B26" name="Range1"/>
-    <protectedRange sqref="B7:B10" name="Range1_2"/>
-    <protectedRange sqref="B12" name="Range1_3"/>
-    <protectedRange sqref="B16:B17" name="Range1_5"/>
-    <protectedRange sqref="B18:B23" name="Range1_6"/>
-    <protectedRange sqref="B27:B30" name="Range1_7"/>
-    <protectedRange sqref="B59:B63" name="Range1_15"/>
-    <protectedRange sqref="B68:B69" name="Range1_16"/>
+    <protectedRange sqref="B47:B52 B69 B58 B5:B6 B17 B13 B15 B28" name="Range1"/>
+    <protectedRange sqref="B7:B12" name="Range1_2"/>
+    <protectedRange sqref="B14" name="Range1_3"/>
+    <protectedRange sqref="B18:B19" name="Range1_5"/>
+    <protectedRange sqref="B20:B25" name="Range1_6"/>
+    <protectedRange sqref="B29:B32" name="Range1_7"/>
+    <protectedRange sqref="B61:B65" name="Range1_15"/>
+    <protectedRange sqref="B70:B71" name="Range1_16"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>